<commit_message>
Adding the desktop version
</commit_message>
<xml_diff>
--- a/grid rows pixels.xlsx
+++ b/grid rows pixels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Coding\MICROVERSE PROGRAM\Module 1\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{8D4514F3-42F2-4E2D-AF0E-10596FDECD78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B139D9F-AF6A-4C97-A14F-C8AE09E2BBB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{F70F8726-ADDE-474E-8077-DE18CC841029}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
-  <si>
-    <t>contenedor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>About</t>
   </si>
@@ -37,6 +34,12 @@
   </si>
   <si>
     <t>card</t>
+  </si>
+  <si>
+    <t>mobile version</t>
+  </si>
+  <si>
+    <t>desktop</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7726AF-5B52-4C30-962F-E6B348BD030D}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +404,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -409,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f>3456-((386+24)*6)</f>
@@ -425,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <f>386+24</f>
@@ -437,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C8" si="0">386+24</f>
@@ -449,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -461,7 +464,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -473,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -485,7 +488,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -497,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1901</v>
@@ -509,6 +512,37 @@
         <v>5357</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>SUM(B12:B15)</f>
+        <v>4556</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>